<commit_message>
WB: rapport fait à adapter et tous les graphes fait ( à dapater)
</commit_message>
<xml_diff>
--- a/tp1_A18_multMat/exemple/Analyses.xlsx
+++ b/tp1_A18_multMat/exemple/Analyses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\inf4705_labs\tp1_A18_multMat\exemple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wajiha\Desktop\inf4705_labs\tp1_A18_multMat\exemple\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C31388-573E-42F5-A25D-E292CB926AD5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F95EF-1E0B-4B6D-BF59-7584BD36E668}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="2" activeTab="3" xr2:uid="{5E549883-D025-457A-8AE3-C662D1935063}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{5E549883-D025-457A-8AE3-C662D1935063}"/>
   </bookViews>
   <sheets>
     <sheet name="Couv" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -733,7 +733,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -768,7 +768,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="510752712"/>
@@ -851,7 +851,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -886,7 +886,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="510757304"/>
@@ -928,7 +928,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -976,7 +976,483 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algo Conventionnel</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphe de synthese'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Couv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12688670166229221"/>
+                  <c:y val="0.17087962962962963"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Graphe de synthese'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Graphe de synthese'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.5590429306030201E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5652179718017498E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1396865844726396E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8119063377380328E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18715407848358112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5119668006896931</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.73655023574824</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95.109519696235637</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>762.52214148044573</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-86D8-4B5F-960D-808793AEE04C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="354367568"/>
+        <c:axId val="354367896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="354367568"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="354367896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="354367896"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="354367568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1027,7 +1503,546 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1562,6 +2577,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C77AE6-0BF8-47CA-A1FF-F765101FFB54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1870,12 +2921,12 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1883,39 +2934,39 @@
         <v>2</v>
       </c>
       <c r="C1">
-        <f>B1*2</f>
+        <f t="shared" ref="C1:J1" si="0">B1*2</f>
         <v>4</v>
       </c>
       <c r="D1">
-        <f>C1*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E1">
-        <f>D1*2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F1">
-        <f>E1*2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="G1">
-        <f>F1*2</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="H1">
-        <f>G1*2</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="I1">
-        <f>H1*2</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="J1">
-        <f>I1*2</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1947,7 +2998,7 @@
         <v>764.00441765785195</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1979,7 +3030,7 @@
         <v>767.15266537666298</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2011,7 +3062,7 @@
         <v>754.37386155128399</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2043,7 +3094,7 @@
         <v>759.20673322677601</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2075,7 +3126,7 @@
         <v>757.88443732261601</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2107,7 +3158,7 @@
         <v>755.69415950775101</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2139,7 +3190,7 @@
         <v>769.18973946571305</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2171,7 +3222,7 @@
         <v>770.75788426399197</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2203,7 +3254,7 @@
         <v>765.69632291793801</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2235,7 +3286,7 @@
         <v>761.26119351387001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2256,23 +3307,23 @@
         <v>2.8119063377380328E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:J13" si="0">AVERAGE(F2:F11)</f>
+        <f t="shared" ref="F13:J13" si="1">AVERAGE(F2:F11)</f>
         <v>0.18715407848358112</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5119668006896931</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.73655023574824</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>95.109519696235637</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>762.52214148044573</v>
       </c>
     </row>
@@ -2290,9 +3341,9 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2300,39 +3351,39 @@
         <v>2</v>
       </c>
       <c r="C1">
-        <f>B1*2</f>
+        <f t="shared" ref="C1:J1" si="0">B1*2</f>
         <v>4</v>
       </c>
       <c r="D1">
-        <f>C1*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E1">
-        <f>D1*2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F1">
-        <f>E1*2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="G1">
-        <f>F1*2</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="H1">
-        <f>G1*2</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="I1">
-        <f>H1*2</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="J1">
-        <f>I1*2</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +3415,7 @@
         <v>4460.1121499538403</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2396,7 +3447,7 @@
         <v>4448.2161841392499</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2428,7 +3479,7 @@
         <v>4416.6805810928299</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2460,7 +3511,7 @@
         <v>4467.9609072208405</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2492,7 +3543,7 @@
         <v>4461.70924353599</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2524,7 +3575,7 @@
         <v>4417.8287050724002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2556,7 +3607,7 @@
         <v>4409.4776251315998</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2588,7 +3639,7 @@
         <v>4454.6364130973798</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2620,7 +3671,7 @@
         <v>9823.9259314536994</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2652,7 +3703,7 @@
         <v>4450.73833417892</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2673,23 +3724,23 @@
         <v>0.26522810459136908</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:J13" si="0">AVERAGE(F2:F11)</f>
+        <f t="shared" ref="F13:J13" si="1">AVERAGE(F2:F11)</f>
         <v>1.835711431503291</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.452552032470649</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>108.28972136974315</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>659.59216358661592</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4981.1286074876743</v>
       </c>
     </row>
@@ -2706,9 +3757,9 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2716,39 +3767,39 @@
         <v>2</v>
       </c>
       <c r="C1">
-        <f>B1*2</f>
+        <f t="shared" ref="C1:J1" si="0">B1*2</f>
         <v>4</v>
       </c>
       <c r="D1">
-        <f>C1*2</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E1">
-        <f>D1*2</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F1">
-        <f>E1*2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="G1">
-        <f>F1*2</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="H1">
-        <f>G1*2</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="I1">
-        <f>H1*2</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="J1">
-        <f>I1*2</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2780,7 +3831,7 @@
         <v>415.24384284019402</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2812,7 +3863,7 @@
         <v>414.68132710456803</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2844,7 +3895,7 @@
         <v>424.82444763183503</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2876,7 +3927,7 @@
         <v>415.137947320938</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2908,7 +3959,7 @@
         <v>423.04885339736899</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2940,7 +3991,7 @@
         <v>416.74557352066</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2972,7 +4023,7 @@
         <v>422.320157289505</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3004,7 +4055,7 @@
         <v>414.64749503135602</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3036,7 +4087,7 @@
         <v>417.94564867019602</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3068,7 +4119,7 @@
         <v>415.21190166473298</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3089,23 +4140,23 @@
         <v>2.881908416748042E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:J13" si="0">AVERAGE(F2:F11)</f>
+        <f t="shared" ref="F13:J13" si="1">AVERAGE(F2:F11)</f>
         <v>0.16761271953582707</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.177203655242915</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3561937093734677</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59.267461752891492</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>417.98071944713536</v>
       </c>
     </row>
@@ -3118,13 +4169,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50119AF-E63F-4751-9976-18D9030322E5}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3138,7 +4189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3155,7 +4206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2*2</f>
         <v>4</v>
@@ -3173,9 +4224,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A11" si="0">A3*2</f>
+        <f t="shared" ref="A4:A10" si="0">A3*2</f>
         <v>8</v>
       </c>
       <c r="B4">
@@ -3191,7 +4242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3209,7 +4260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3227,7 +4278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -3245,7 +4296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3263,7 +4314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>256</v>
@@ -3281,7 +4332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>512</v>

</xml_diff>